<commit_message>
new implementation of actual dpackjar table inside the zz3 popup on driggsman page - could be heavy or mess up page speed etc
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/370 sko related but different - gbp worker fb - listings/kr exports stuff 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/370 sko related but different - gbp worker fb - listings/kr exports stuff 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/370 sko related but different - gbp worker fb - listings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468D4D42-3E48-0B43-8394-9960B6416A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B291A601-79B0-A643-B988-4B704C875934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{D1862B61-F6C7-EA47-BF6E-DA13A3862256}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>